<commit_message>
Corregida plantilla de configuracion, no mostraba las listas de seleccion Mejorada redireccion por acceso no permitidos a las funciones (muestra error 404) Eliminada la opcion enviar por de la plantilla (se asume siempre envio POST) Agregada ventana de login, el usuario de be crear una hoja con el nombre reservado ZC_Login
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Paises" sheetId="3" r:id="rId1"/>
     <sheet name="Usuarios" sheetId="1" r:id="rId2"/>
-    <sheet name="ZeroCode" sheetId="2" r:id="rId3"/>
+    <sheet name="ZeroCode" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="ZC_Login" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -26,7 +27,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color theme="1"/>
+            <color indexed="8"/>
             <rFont val="Liberation Sans"/>
           </rPr>
           <t>Tipo de elemento a crear</t>
@@ -38,7 +39,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color theme="1"/>
+            <color indexed="8"/>
             <rFont val="Liberation Sans"/>
           </rPr>
           <t>Nombre del elemento, este se mostrara al cliente, ademas es el nombre del campo en la base de datos. Los espacios se reemplazan por _</t>
@@ -60,7 +61,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color theme="1"/>
+            <color indexed="8"/>
             <rFont val="Liberation Sans"/>
           </rPr>
           <t>Tipo de elemento a crear</t>
@@ -72,7 +73,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color theme="1"/>
+            <color indexed="8"/>
             <rFont val="Liberation Sans"/>
           </rPr>
           <t>Nombre del elemento, este se mostrara al cliente, ademas es el nombre del campo en la base de datos. Los espacios se reemplazan por _</t>
@@ -94,7 +95,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color theme="1"/>
+            <color indexed="8"/>
             <rFont val="Liberation Sans"/>
           </rPr>
           <t>Input:text</t>
@@ -106,7 +107,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color theme="1"/>
+            <color indexed="8"/>
             <rFont val="Liberation Sans"/>
           </rPr>
           <t>Input:radio</t>
@@ -118,7 +119,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color theme="1"/>
+            <color indexed="8"/>
             <rFont val="Liberation Sans"/>
           </rPr>
           <t>Input:checkbox</t>
@@ -130,7 +131,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color theme="1"/>
+            <color indexed="8"/>
             <rFont val="Liberation Sans"/>
           </rPr>
           <t>Input:select</t>
@@ -142,7 +143,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color theme="1"/>
+            <color indexed="8"/>
             <rFont val="Liberation Sans"/>
           </rPr>
           <t>Input:hidden</t>
@@ -154,7 +155,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color theme="1"/>
+            <color indexed="8"/>
             <rFont val="Liberation Sans"/>
           </rPr>
           <t>button:button</t>
@@ -165,27 +166,52 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Liberation Sans"/>
+          </rPr>
+          <t>Tipo de elemento a crear</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Liberation Sans"/>
+          </rPr>
+          <t>Nombre del elemento, este se mostrara al cliente, ademas es el nombre del campo en la base de datos. Los espacios se reemplazan por _</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="61">
   <si>
     <t>Nombre Formulario</t>
   </si>
   <si>
-    <t>Se envia</t>
-  </si>
-  <si>
     <t>Tipo de servicio</t>
   </si>
   <si>
     <t>Se guardara en</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>POST</t>
-  </si>
-  <si>
     <t>SOAP</t>
   </si>
   <si>
@@ -324,15 +350,9 @@
     <t>Es obligatorio</t>
   </si>
   <si>
-    <t>Modos de envio</t>
-  </si>
-  <si>
     <t>Tipo Web Service</t>
   </si>
   <si>
-    <t>GET</t>
-  </si>
-  <si>
     <t>REST</t>
   </si>
   <si>
@@ -358,6 +378,12 @@
   </si>
   <si>
     <t>Paises::nombre</t>
+  </si>
+  <si>
+    <t>Usuarios</t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
 </sst>
 </file>
@@ -371,6 +397,11 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Liberation Sans"/>
     </font>
     <font>
@@ -392,11 +423,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Liberation Sans"/>
     </font>
   </fonts>
@@ -425,18 +451,18 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -745,7 +771,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -773,76 +799,106 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
+          <x14:formula1>
+            <xm:f>ZeroCode!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>A4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de webservice" prompt="Tipo de conexion al servidor">
+          <x14:formula1>
+            <xm:f>ZeroCode!$D$2:$D$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Base de datos" prompt="Base de datos utilizar, se puede configurar por formulario">
+          <x14:formula1>
+            <xm:f>ZeroCode!$E$2:$E$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Es un campo obligatorio?" prompt="Si el campo es obligatorio, seleccione la opcion si, de lo contrario el campo no es obligatorio">
+          <x14:formula1>
+            <xm:f>ZeroCode!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de dato" prompt="Selecciona el tipo de dato a recibir">
+          <x14:formula1>
+            <xm:f>ZeroCode!$B$2:$B$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -850,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -877,71 +933,65 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -950,30 +1000,30 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -982,118 +1032,275 @@
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>37</v>
-      </c>
       <c r="K7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" t="s">
         <v>38</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>22</v>
       </c>
       <c r="G10">
         <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G11">
         <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
+          <x14:formula1>
+            <xm:f>ZeroCode!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>A4:A11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de webservice" prompt="Tipo de conexion al servidor">
+          <x14:formula1>
+            <xm:f>ZeroCode!$D$2:$D$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Base de datos" prompt="Base de datos utilizar, se puede configurar por formulario">
+          <x14:formula1>
+            <xm:f>ZeroCode!$E$2:$E$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Es un campo obligatorio?" prompt="Si el campo es obligatorio, seleccione la opcion si, de lo contrario el campo no es obligatorio">
+          <x14:formula1>
+            <xm:f>ZeroCode!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E4:E11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de dato" prompt="Selecciona el tipo de dato a recibir">
+          <x14:formula1>
+            <xm:f>ZeroCode!$B$2:$B$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4:C11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="15.125" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1106,133 +1313,161 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.125" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="3" width="10.625" customWidth="1"/>
-    <col min="4" max="4" width="13.375" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" t="s">
+    <row r="1" spans="1:11" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F4">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8" t="s">
-        <v>45</v>
+        <v>19</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Base de datos" prompt="Base de datos utilizar, se puede configurar por formulario">
+          <x14:formula1>
+            <xm:f>ZeroCode!$E$2:$E$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de webservice" prompt="Tipo de conexion al servidor">
+          <x14:formula1>
+            <xm:f>ZeroCode!$D$2:$D$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de dato" prompt="Selecciona el tipo de dato a recibir">
+          <x14:formula1>
+            <xm:f>ZeroCode!$B$2:$B$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4:C5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Es un campo obligatorio?" prompt="Si el campo es obligatorio, seleccione la opcion si, de lo contrario el campo no es obligatorio">
+          <x14:formula1>
+            <xm:f>ZeroCode!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>E4:E5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
+          <x14:formula1>
+            <xm:f>ZeroCode!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>A4:A5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Creadas plantillas para el manejo de usuarios Agregada funcion para centralizar el reemplzao de caracteres especiales
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="3"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Paises" sheetId="3" r:id="rId1"/>
-    <sheet name="Usuarios" sheetId="1" r:id="rId2"/>
+    <sheet name="Clientes" sheetId="1" r:id="rId2"/>
     <sheet name="ZeroCode" sheetId="2" state="hidden" r:id="rId3"/>
-    <sheet name="ZC_Login" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -166,42 +165,8 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="A3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="8"/>
-            <rFont val="Liberation Sans"/>
-          </rPr>
-          <t>Tipo de elemento a crear</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="8"/>
-            <rFont val="Liberation Sans"/>
-          </rPr>
-          <t>Nombre del elemento, este se mostrara al cliente, ademas es el nombre del campo en la base de datos. Los espacios se reemplazan por _</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>Nombre Formulario</t>
   </si>
@@ -254,9 +219,6 @@
     <t>Caja</t>
   </si>
   <si>
-    <t>Usuario</t>
-  </si>
-  <si>
     <t>texto</t>
   </si>
   <si>
@@ -287,12 +249,6 @@
     <t>Circulo</t>
   </si>
   <si>
-    <t>Genero</t>
-  </si>
-  <si>
-    <t>F=Mujer,M=Hombre</t>
-  </si>
-  <si>
     <t>Listado</t>
   </si>
   <si>
@@ -320,21 +276,12 @@
     <t>1=Si</t>
   </si>
   <si>
-    <t>Fecha</t>
-  </si>
-  <si>
     <t>fecha</t>
   </si>
   <si>
-    <t>Clave</t>
-  </si>
-  <si>
     <t>clave</t>
   </si>
   <si>
-    <t>Y la seguridad...</t>
-  </si>
-  <si>
     <t>Observaciones</t>
   </si>
   <si>
@@ -380,10 +327,16 @@
     <t>Paises::nombre</t>
   </si>
   <si>
-    <t>Usuarios</t>
-  </si>
-  <si>
-    <t>Login</t>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>F=Natural,M=Juridica</t>
+  </si>
+  <si>
+    <t>Tipo cliente</t>
+  </si>
+  <si>
+    <t>Fecha registro</t>
   </si>
 </sst>
 </file>
@@ -802,7 +755,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -851,13 +804,13 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -904,10 +857,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -936,7 +889,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -985,13 +938,13 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -1000,13 +953,13 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1014,16 +967,16 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -1032,67 +985,67 @@
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" t="s">
-        <v>34</v>
-      </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1100,13 +1053,13 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1114,35 +1067,15 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="G10">
-        <v>15</v>
-      </c>
-      <c r="H10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11">
         <v>100</v>
       </c>
     </row>
@@ -1156,12 +1089,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
-          <x14:formula1>
-            <xm:f>ZeroCode!$A$2:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>A4:A11</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de webservice" prompt="Tipo de conexion al servidor">
           <x14:formula1>
             <xm:f>ZeroCode!$D$2:$D$3</xm:f>
@@ -1174,17 +1101,23 @@
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
+          <x14:formula1>
+            <xm:f>ZeroCode!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>A4:A10</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Es un campo obligatorio?" prompt="Si el campo es obligatorio, seleccione la opcion si, de lo contrario el campo no es obligatorio">
           <x14:formula1>
             <xm:f>ZeroCode!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:E11</xm:sqref>
+          <xm:sqref>E4:E10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de dato" prompt="Selecciona el tipo de dato a recibir">
           <x14:formula1>
             <xm:f>ZeroCode!$B$2:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C4:C11</xm:sqref>
+          <xm:sqref>C4:C10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1211,16 +1144,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1231,10 +1164,10 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -1245,62 +1178,62 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="B8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1311,163 +1244,4 @@
   </headerFooter>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Base de datos" prompt="Base de datos utilizar, se puede configurar por formulario">
-          <x14:formula1>
-            <xm:f>ZeroCode!$E$2:$E$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de webservice" prompt="Tipo de conexion al servidor">
-          <x14:formula1>
-            <xm:f>ZeroCode!$D$2:$D$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de dato" prompt="Selecciona el tipo de dato a recibir">
-          <x14:formula1>
-            <xm:f>ZeroCode!$B$2:$B$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>C4:C5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Es un campo obligatorio?" prompt="Si el campo es obligatorio, seleccione la opcion si, de lo contrario el campo no es obligatorio">
-          <x14:formula1>
-            <xm:f>ZeroCode!$C$2:$C$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>E4:E5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
-          <x14:formula1>
-            <xm:f>ZeroCode!$A$2:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>A4:A5</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Cuando el usuario tiene una sesion abierta, se habilita la pagina de inicio Se minimizan las opciones a diligenciar en la plantilla de configuracion Agregada mejora #33 Agregadas mejoras visuales a los formulario
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855"/>
   </bookViews>
   <sheets>
     <sheet name="Paises" sheetId="3" r:id="rId1"/>
@@ -166,12 +166,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t>Nombre Formulario</t>
-  </si>
-  <si>
-    <t>Tipo de servicio</t>
   </si>
   <si>
     <t>Se guardara en</t>
@@ -723,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -746,71 +743,59 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -859,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -880,71 +865,59 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -953,30 +926,30 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>20</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -985,95 +958,95 @@
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
         <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>31</v>
-      </c>
       <c r="K7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="K8" t="s">
         <v>34</v>
-      </c>
-      <c r="K8" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10">
         <v>100</v>
@@ -1144,96 +1117,96 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregados tipo de datos fecha y fecha hora, mejora #41 Corregido problema en cajas tipo fecha Por defecto ningun campo es obligatorio
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Paises" sheetId="3" r:id="rId1"/>
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t>Nombre Formulario</t>
   </si>
@@ -334,6 +334,21 @@
   </si>
   <si>
     <t>Fecha registro</t>
+  </si>
+  <si>
+    <t>fecha hora</t>
+  </si>
+  <si>
+    <t>hora</t>
+  </si>
+  <si>
+    <t>Hora registro</t>
+  </si>
+  <si>
+    <t>Ultima actualizacion</t>
+  </si>
+  <si>
+    <t>Pagina web</t>
   </si>
 </sst>
 </file>
@@ -720,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -830,7 +845,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de dato" prompt="Selecciona el tipo de dato a recibir">
           <x14:formula1>
-            <xm:f>ZeroCode!$B$2:$B$8</xm:f>
+            <xm:f>ZeroCode!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>C4</xm:sqref>
         </x14:dataValidation>
@@ -842,10 +857,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -983,42 +998,36 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
       </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1026,13 +1035,16 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>33</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1040,16 +1052,49 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10">
-        <v>100</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1078,19 +1123,19 @@
           <x14:formula1>
             <xm:f>ZeroCode!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>A4:A10</xm:sqref>
+          <xm:sqref>A13 A4:A6 A8:A10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Es un campo obligatorio?" prompt="Si el campo es obligatorio, seleccione la opcion si, de lo contrario el campo no es obligatorio">
           <x14:formula1>
             <xm:f>ZeroCode!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:E10</xm:sqref>
+          <xm:sqref>E4:E6 E8:E13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de dato" prompt="Selecciona el tipo de dato a recibir">
           <x14:formula1>
-            <xm:f>ZeroCode!$B$2:$B$8</xm:f>
+            <xm:f>ZeroCode!$B$2:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C4:C10</xm:sqref>
+          <xm:sqref>C4:C13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1100,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1137,7 +1182,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1165,7 +1210,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1173,7 +1218,7 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
         <v>43</v>
@@ -1184,7 +1229,7 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
         <v>44</v>
@@ -1195,7 +1240,7 @@
         <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
         <v>47</v>
@@ -1203,10 +1248,20 @@
     </row>
     <row r="8" spans="1:5">
       <c r="B8" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregadas validaciones del lado servidor para datos fecha y fecha hora Mejorado ejemplo, agregando los nuevos tipos de campo
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -327,9 +327,6 @@
     <t>Clientes</t>
   </si>
   <si>
-    <t>F=Natural,M=Juridica</t>
-  </si>
-  <si>
     <t>Tipo cliente</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>Pagina web</t>
+  </si>
+  <si>
+    <t>N=Natural,J=Juridica</t>
   </si>
 </sst>
 </file>
@@ -859,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -981,7 +981,7 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -993,7 +993,7 @@
         <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1001,7 +1001,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
@@ -1052,7 +1052,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
@@ -1066,10 +1066,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1077,10 +1077,10 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1240,7 +1240,7 @@
         <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
         <v>47</v>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Agregada hoja de configuracion al excel Se agregan variables para colocar las URL de los servicios (aun no se usan) Se agrega la opcion de colocar valor por defecto
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -7,9 +7,10 @@
     <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Paises" sheetId="3" r:id="rId1"/>
-    <sheet name="Clientes" sheetId="1" r:id="rId2"/>
-    <sheet name="ZeroCode" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Config" sheetId="4" r:id="rId1"/>
+    <sheet name="Paises" sheetId="3" r:id="rId2"/>
+    <sheet name="Clientes" sheetId="1" r:id="rId3"/>
+    <sheet name="ZeroCode" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -18,10 +19,163 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Farfan</author>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Este nombre se muestra en el formulario</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tipo de motor de base de datos que se usa para almacenar los datos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+URL donde se encuentra el WS a consumir, es del tipo:
+soap|http://path/ws
+rest|http://path/ws</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+URL donde se encuentra el WS a consumir, es del tipo:
+soap|http://path/ws
+rest|http://path/ws</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+URL donde se encuentra el WS a consumir, es del tipo:
+soap|http://path/ws
+rest|http://path/ws</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+URL donde se encuentra el WS a consumir, es del tipo:
+soap|http://path/ws
+rest|http://path/ws</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="1">
       <text>
         <r>
           <rPr>
@@ -33,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="1">
       <text>
         <r>
           <rPr>
@@ -166,7 +320,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="89">
   <si>
     <t>Nombre Formulario</t>
   </si>
@@ -349,6 +503,90 @@
   </si>
   <si>
     <t>N=Natural,J=Juridica</t>
+  </si>
+  <si>
+    <t>WS Agregar</t>
+  </si>
+  <si>
+    <t>Motor BD</t>
+  </si>
+  <si>
+    <t>WS Consultar</t>
+  </si>
+  <si>
+    <t>WS Borrar</t>
+  </si>
+  <si>
+    <t>WS Eliminar</t>
+  </si>
+  <si>
+    <t>Por defecto es</t>
+  </si>
+  <si>
+    <t>Nombre campo BD</t>
+  </si>
+  <si>
+    <t>http://agregar</t>
+  </si>
+  <si>
+    <t>http://consultar</t>
+  </si>
+  <si>
+    <t>http://borrar</t>
+  </si>
+  <si>
+    <t>http://eliminar</t>
+  </si>
+  <si>
+    <t>PaNombre</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Se necesitan caracteres</t>
+  </si>
+  <si>
+    <t>Por favor coloca el nombre</t>
+  </si>
+  <si>
+    <t>Ojo la longitud minima</t>
+  </si>
+  <si>
+    <t>Supera la longitud maxima</t>
+  </si>
+  <si>
+    <t>Valores</t>
+  </si>
+  <si>
+    <t>BD Servidor</t>
+  </si>
+  <si>
+    <t>BD Puerto</t>
+  </si>
+  <si>
+    <t>BD Esquema</t>
+  </si>
+  <si>
+    <t>BD Usuario</t>
+  </si>
+  <si>
+    <t>BD Clave</t>
+  </si>
+  <si>
+    <t>localhost</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>1q2w3e4r</t>
+  </si>
+  <si>
+    <t>Registros por pagina</t>
+  </si>
+  <si>
+    <t>pruebas</t>
   </si>
 </sst>
 </file>
@@ -358,7 +596,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-240A]#,##0.00;[Red]&quot;(&quot;[$$-240A]#,##0.00&quot;)&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,6 +628,25 @@
       <color rgb="FFFFFFFF"/>
       <name val="Liberation Sans"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Liberation Sans"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -414,7 +671,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment horizontal="center"/>
@@ -424,14 +681,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Heading" xfId="1"/>
     <cellStyle name="Heading1" xfId="2"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Result" xfId="3"/>
     <cellStyle name="Result2" xfId="4"/>
@@ -732,11 +992,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="3" max="3" width="15.125" customWidth="1"/>
+    <col min="4" max="4" width="14.25" customWidth="1"/>
+    <col min="5" max="5" width="14.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2">
+        <v>3306</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -745,26 +1071,58 @@
     <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15">
+    <row r="1" spans="1:13" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -775,16 +1133,16 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>11</v>
@@ -796,10 +1154,16 @@
         <v>13</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>78</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -809,33 +1173,57 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
           <x14:formula1>
             <xm:f>ZeroCode!$A$2:$A$7</xm:f>
           </x14:formula1>
           <xm:sqref>A4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de webservice" prompt="Tipo de conexion al servidor">
-          <x14:formula1>
-            <xm:f>ZeroCode!$D$2:$D$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Base de datos" prompt="Base de datos utilizar, se puede configurar por formulario">
           <x14:formula1>
             <xm:f>ZeroCode!$E$2:$E$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
+          <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Es un campo obligatorio?" prompt="Si el campo es obligatorio, seleccione la opcion si, de lo contrario el campo no es obligatorio">
           <x14:formula1>
@@ -855,12 +1243,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1143,7 +1531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Agregado parametros de charset y collation a la configuracion desde la hoja de calculo
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="4" r:id="rId1"/>
     <sheet name="Paises" sheetId="3" r:id="rId2"/>
     <sheet name="Clientes" sheetId="1" r:id="rId3"/>
-    <sheet name="ZeroCode" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="ZeroCode" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -320,7 +320,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
   <si>
     <t>Nombre Formulario</t>
   </si>
@@ -587,6 +587,33 @@
   </si>
   <si>
     <t>pruebas</t>
+  </si>
+  <si>
+    <t>BD Motor</t>
+  </si>
+  <si>
+    <t>BD Charset</t>
+  </si>
+  <si>
+    <t>BD Collation</t>
+  </si>
+  <si>
+    <t>Charset</t>
+  </si>
+  <si>
+    <t>Collation</t>
+  </si>
+  <si>
+    <t>utf8</t>
+  </si>
+  <si>
+    <t>utf8_general_ci</t>
+  </si>
+  <si>
+    <t>latin1</t>
+  </si>
+  <si>
+    <t>latin1_swedish_ci</t>
   </si>
 </sst>
 </file>
@@ -596,7 +623,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-240A]#,##0.00;[Red]&quot;(&quot;[$$-240A]#,##0.00&quot;)&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -647,6 +674,12 @@
       <color theme="10"/>
       <name val="Liberation Sans"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -683,10 +716,11 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Heading" xfId="1"/>
@@ -993,67 +1027,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="15.125" customWidth="1"/>
-    <col min="4" max="4" width="14.25" customWidth="1"/>
-    <col min="5" max="5" width="14.75" customWidth="1"/>
+    <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="5" width="14.25" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>84</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>3306</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>88</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>85</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Base de datos" prompt="Base de datos utilizar, se puede configurar por formulario">
+          <x14:formula1>
+            <xm:f>ZeroCode!$E$2:$E$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>ZeroCode!$F$2:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>ZeroCode!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1061,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1533,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1548,7 +1621,7 @@
     <col min="5" max="5" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -1564,8 +1637,14 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1581,8 +1660,14 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1592,8 +1677,14 @@
       <c r="C3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1601,7 +1692,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1612,7 +1703,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1623,7 +1714,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -1634,7 +1725,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="B8" t="s">
         <v>55</v>
       </c>
@@ -1642,22 +1733,23 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="B9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="B10" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Eliminado el formato plano para la creacion de proyectos Quitar Notice y Warning para poder trabajar con error_reporting = E_ALL
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="4" r:id="rId1"/>
     <sheet name="Paises" sheetId="3" r:id="rId2"/>
     <sheet name="Clientes" sheetId="1" r:id="rId3"/>
-    <sheet name="ZeroCode" sheetId="2" r:id="rId4"/>
+    <sheet name="ZeroCode" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -233,6 +233,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="A14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Liberation Sans"/>
+          </rPr>
+          <t>Tipo de elemento a crear</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Liberation Sans"/>
+          </rPr>
+          <t>Nombre del elemento, este se mostrara al cliente, ademas es el nombre del campo en la base de datos. Los espacios se reemplazan por _</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -320,7 +344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
   <si>
     <t>Nombre Formulario</t>
   </si>
@@ -362,9 +386,6 @@
   </si>
   <si>
     <t>Mensaje de error longitud maxima</t>
-  </si>
-  <si>
-    <t>Posibles valores</t>
   </si>
   <si>
     <t>Caja</t>
@@ -1029,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1047,28 +1068,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1076,29 +1097,29 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2">
         <v>3306</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
         <v>85</v>
-      </c>
-      <c r="F2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1135,7 +1156,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1150,7 +1171,7 @@
     <col min="8" max="8" width="29.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1160,39 +1181,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15">
@@ -1212,66 +1233,66 @@
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" t="s">
         <v>73</v>
-      </c>
-      <c r="G4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" t="s">
-        <v>75</v>
       </c>
       <c r="I4" t="s">
         <v>76</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L4" t="s">
-        <v>72</v>
-      </c>
-      <c r="M4">
-        <v>10</v>
+        <v>74</v>
+      </c>
+      <c r="K4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1318,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1329,25 +1350,27 @@
     <col min="1" max="1" width="21.75" customWidth="1"/>
     <col min="2" max="2" width="27.125" customWidth="1"/>
     <col min="3" max="3" width="16.75" customWidth="1"/>
-    <col min="4" max="4" width="23.75" customWidth="1"/>
-    <col min="5" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="18.75" customWidth="1"/>
-    <col min="8" max="9" width="29.375" customWidth="1"/>
-    <col min="10" max="10" width="29.75" customWidth="1"/>
-    <col min="11" max="11" width="14.75" customWidth="1"/>
+    <col min="4" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="18.75" customWidth="1"/>
+    <col min="7" max="8" width="29.375" customWidth="1"/>
+    <col min="9" max="9" width="29.75" customWidth="1"/>
+    <col min="10" max="10" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15">
+    <row r="1" spans="1:13" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1358,7 +1381,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
@@ -1367,197 +1390,204 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
       </c>
       <c r="F4">
         <v>5</v>
       </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
       <c r="I4" t="s">
         <v>19</v>
       </c>
       <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
+      <c r="D5">
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
-      <c r="G5">
-        <v>20</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
         <v>53</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="K6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="L13" t="s">
         <v>33</v>
       </c>
-      <c r="G9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="K13" t="s">
-        <v>34</v>
-      </c>
-    </row>
+    </row>
+    <row r="14" spans="1:13"/>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <headerFooter>
@@ -1590,7 +1620,7 @@
           <x14:formula1>
             <xm:f>ZeroCode!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:E6 E8:E13</xm:sqref>
+          <xm:sqref>E4:E6 E8:E10 D23:D25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de dato" prompt="Selecciona el tipo de dato a recibir">
           <x14:formula1>
@@ -1623,36 +1653,36 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
         <v>92</v>
-      </c>
-      <c r="G1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -1661,86 +1691,86 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" t="s">
         <v>96</v>
-      </c>
-      <c r="G3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambiados creacion de plantillas para facilitar las actualizaciones Se cambia el nombre de los elementos utilizados en los formulario
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="4" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Clientes" sheetId="1" r:id="rId3"/>
     <sheet name="ZeroCode" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -418,12 +418,6 @@
     <t>Al menos 10</t>
   </si>
   <si>
-    <t>Circulo</t>
-  </si>
-  <si>
-    <t>Listado</t>
-  </si>
-  <si>
     <t>Pais</t>
   </si>
   <si>
@@ -436,9 +430,6 @@
     <t>y el pais?</t>
   </si>
   <si>
-    <t>Cuadrado</t>
-  </si>
-  <si>
     <t>Recibir publicidad</t>
   </si>
   <si>
@@ -635,12 +626,21 @@
   </si>
   <si>
     <t>latin1_swedish_ci</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Lista</t>
+  </si>
+  <si>
+    <t>Checkbox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-240A]#,##0.00;[Red]&quot;(&quot;[$$-240A]#,##0.00&quot;)&quot;"/>
   </numFmts>
@@ -746,7 +746,7 @@
   <cellStyles count="6">
     <cellStyle name="Heading" xfId="1"/>
     <cellStyle name="Heading1" xfId="2"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Result" xfId="3"/>
     <cellStyle name="Result2" xfId="4"/>
@@ -762,7 +762,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -836,7 +836,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -871,7 +870,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1047,14 +1045,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.125" customWidth="1"/>
@@ -1068,28 +1066,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1097,24 +1095,24 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <v>3306</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1152,14 +1150,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
@@ -1181,39 +1179,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15">
@@ -1236,7 +1234,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -1251,10 +1249,10 @@
         <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1262,7 +1260,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -1277,22 +1275,22 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" t="s">
         <v>72</v>
       </c>
-      <c r="H4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" t="s">
-        <v>76</v>
-      </c>
-      <c r="J4" t="s">
-        <v>74</v>
-      </c>
-      <c r="K4" t="s">
-        <v>75</v>
-      </c>
       <c r="M4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1304,8 +1302,8 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId5"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+  <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
           <x14:formula1>
@@ -1338,14 +1336,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="21.75" customWidth="1"/>
     <col min="2" max="2" width="27.125" customWidth="1"/>
@@ -1367,7 +1365,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15">
@@ -1390,7 +1388,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -1405,10 +1403,10 @@
         <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1416,7 +1414,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -1468,10 +1466,10 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -1483,7 +1481,7 @@
         <v>16</v>
       </c>
       <c r="L6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1491,33 +1489,33 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1525,16 +1523,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D9">
         <v>100</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1542,10 +1540,10 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -1556,10 +1554,10 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1567,24 +1565,24 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" t="s">
         <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:13"/>
@@ -1595,8 +1593,8 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+  <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de webservice" prompt="Tipo de conexion al servidor">
           <x14:formula1>
@@ -1635,14 +1633,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>
@@ -1653,25 +1651,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
         <v>38</v>
-      </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75">
@@ -1691,32 +1689,32 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -1724,53 +1722,53 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambiado el nombre de la pagina de login de Zlogin => Login Se centraliza el manejo del nombre ZC_PAGINA_LOGIN Los id (de base de datos y elmentos html) se manejan como son ingresados en Excel, es decir preservan minusculas y mayusculas, solo se cambian caracteres especiales Cambiada funcion que determina la extension del archivo, se utiliza la de PHP Mejorado manejo en la asignacion de errores, diferencia JSON de String para mostrar los errores Eliminada funcion IsJsonString en zc.js, ya no se usa
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="4" r:id="rId1"/>
@@ -487,9 +487,6 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t>Paises::nombre</t>
-  </si>
-  <si>
     <t>Clientes</t>
   </si>
   <si>
@@ -635,12 +632,15 @@
   </si>
   <si>
     <t>Checkbox</t>
+  </si>
+  <si>
+    <t>Paises::PaNombre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-240A]#,##0.00;[Red]&quot;(&quot;[$$-240A]#,##0.00&quot;)&quot;"/>
   </numFmts>
@@ -746,7 +746,7 @@
   <cellStyles count="6">
     <cellStyle name="Heading" xfId="1"/>
     <cellStyle name="Heading1" xfId="2"/>
-    <cellStyle name="Hipervínculo" xfId="5" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Result" xfId="3"/>
     <cellStyle name="Result2" xfId="4"/>
@@ -762,7 +762,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -836,6 +836,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -870,6 +871,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1045,14 +1047,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.125" customWidth="1"/>
@@ -1066,28 +1068,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1095,24 +1097,24 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2">
         <v>3306</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
         <v>81</v>
-      </c>
-      <c r="F2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1150,14 +1152,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
@@ -1179,19 +1181,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1202,16 +1204,16 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15">
@@ -1234,7 +1236,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -1249,10 +1251,10 @@
         <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1275,22 +1277,22 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
         <v>69</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" t="s">
         <v>70</v>
       </c>
-      <c r="I4" t="s">
-        <v>73</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>71</v>
       </c>
-      <c r="K4" t="s">
-        <v>72</v>
-      </c>
       <c r="M4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1302,8 +1304,8 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId5"/>
-  <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
           <x14:formula1>
@@ -1336,14 +1338,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="21.75" customWidth="1"/>
     <col min="2" max="2" width="27.125" customWidth="1"/>
@@ -1365,7 +1367,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15">
@@ -1388,7 +1390,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -1403,10 +1405,10 @@
         <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1466,10 +1468,10 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -1481,7 +1483,7 @@
         <v>16</v>
       </c>
       <c r="L6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1489,7 +1491,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
@@ -1497,7 +1499,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -1515,7 +1517,7 @@
         <v>27</v>
       </c>
       <c r="L8" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1540,7 +1542,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
@@ -1554,10 +1556,10 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1565,15 +1567,15 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
@@ -1593,8 +1595,8 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId1"/>
-  <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de webservice" prompt="Tipo de conexion al servidor">
           <x14:formula1>
@@ -1633,14 +1635,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>
@@ -1666,10 +1668,10 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
         <v>88</v>
-      </c>
-      <c r="G1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75">
@@ -1689,15 +1691,15 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -1706,15 +1708,15 @@
         <v>29</v>
       </c>
       <c r="F3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" t="s">
         <v>92</v>
-      </c>
-      <c r="G3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -1722,7 +1724,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
@@ -1747,7 +1749,7 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
         <v>43</v>
@@ -1755,7 +1757,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Se deja del lado servidor la validacion de datos y validacion de filtros, se quita en el modelo cliente Se corrije error a ejecutar la acciones precargar, loguear y ajax directamente WS Se agrega validacion para la crear la accion "ajax", solo si el formulario tiene joins con otras tablas se crea #59
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="4" r:id="rId1"/>
@@ -344,7 +344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="89">
   <si>
     <t>Nombre Formulario</t>
   </si>
@@ -514,37 +514,13 @@
     <t>N=Natural,J=Juridica</t>
   </si>
   <si>
-    <t>WS Agregar</t>
-  </si>
-  <si>
     <t>Motor BD</t>
   </si>
   <si>
-    <t>WS Consultar</t>
-  </si>
-  <si>
-    <t>WS Borrar</t>
-  </si>
-  <si>
-    <t>WS Eliminar</t>
-  </si>
-  <si>
     <t>Por defecto es</t>
   </si>
   <si>
     <t>Nombre campo BD</t>
-  </si>
-  <si>
-    <t>http://agregar</t>
-  </si>
-  <si>
-    <t>http://consultar</t>
-  </si>
-  <si>
-    <t>http://borrar</t>
-  </si>
-  <si>
-    <t>http://eliminar</t>
   </si>
   <si>
     <t>PaNombre</t>
@@ -640,11 +616,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-240A]#,##0.00;[Red]&quot;(&quot;[$$-240A]#,##0.00&quot;)&quot;"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -690,12 +666,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
@@ -725,7 +695,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment horizontal="center"/>
@@ -735,18 +705,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
     <cellStyle name="Heading1" xfId="2"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Result" xfId="3"/>
     <cellStyle name="Result2" xfId="4"/>
@@ -762,7 +729,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -836,7 +803,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -871,7 +837,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1047,14 +1012,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.125" customWidth="1"/>
@@ -1068,28 +1033,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1097,24 +1062,24 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C2">
         <v>3306</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1152,14 +1117,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
@@ -1181,19 +1146,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1203,18 +1156,6 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="3" spans="1:13" ht="15">
       <c r="A3" s="1" t="s">
@@ -1236,7 +1177,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -1251,10 +1192,10 @@
         <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1277,35 +1218,29 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="I4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="J4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="M4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="F2" r:id="rId4"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId5"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+  <legacyDrawing r:id="rId1"/>
+  <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
           <x14:formula1>
@@ -1338,14 +1273,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="21.75" customWidth="1"/>
     <col min="2" max="2" width="27.125" customWidth="1"/>
@@ -1390,7 +1325,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -1405,10 +1340,10 @@
         <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1468,7 +1403,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
@@ -1499,7 +1434,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -1517,7 +1452,7 @@
         <v>27</v>
       </c>
       <c r="L8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1575,7 +1510,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
@@ -1595,8 +1530,8 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+  <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de webservice" prompt="Tipo de conexion al servidor">
           <x14:formula1>
@@ -1635,14 +1570,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>
@@ -1668,10 +1603,10 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75">
@@ -1690,16 +1625,16 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>90</v>
+      <c r="F2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -1708,15 +1643,15 @@
         <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -1724,7 +1659,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Agregadas nuevas caracteristicas posibles en el sistema, como parametros en la hoja de calculo
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="1"/>
@@ -206,10 +206,167 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Farfan</author>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+URL donde se encuentra el WS a consumir, es del tipo:
+soap|http://path/ws
+rest|http://path/ws</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+URL donde se encuentra el WS a consumir, es del tipo:
+soap|http://path/ws
+rest|http://path/ws</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+URL donde se encuentra el WS a consumir, es del tipo:
+soap|http://path/ws
+rest|http://path/ws</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+URL donde se encuentra el WS a consumir, es del tipo:
+soap|http://path/ws
+rest|http://path/ws</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+URL donde se encuentra el WS a consumir, es del tipo:
+soap|http://path/ws
+rest|http://path/ws</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+URL donde se encuentra el WS a consumir, es del tipo:
+soap|http://path/ws
+rest|http://path/ws</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="1">
       <text>
         <r>
           <rPr>
@@ -221,7 +378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="1">
       <text>
         <r>
           <rPr>
@@ -233,7 +390,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="0">
+    <comment ref="A14" authorId="1">
       <text>
         <r>
           <rPr>
@@ -245,7 +402,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0">
+    <comment ref="B14" authorId="1">
       <text>
         <r>
           <rPr>
@@ -344,7 +501,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="97">
   <si>
     <t>Nombre Formulario</t>
   </si>
@@ -611,16 +768,40 @@
   </si>
   <si>
     <t>Paises::PaNombre</t>
+  </si>
+  <si>
+    <t>WS Agregar</t>
+  </si>
+  <si>
+    <t>WS Buscar</t>
+  </si>
+  <si>
+    <t>WS Modificar</t>
+  </si>
+  <si>
+    <t>WS Borrar</t>
+  </si>
+  <si>
+    <t>WS Ajax</t>
+  </si>
+  <si>
+    <t>WS Precargar</t>
+  </si>
+  <si>
+    <t>Nombre tabla</t>
+  </si>
+  <si>
+    <t>t_paises</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-240A]#,##0.00;[Red]&quot;(&quot;[$$-240A]#,##0.00&quot;)&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -665,12 +846,6 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -706,10 +881,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -729,7 +903,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -803,6 +977,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -837,6 +1012,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1012,14 +1188,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.125" customWidth="1"/>
@@ -1117,14 +1293,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
@@ -1148,6 +1324,9 @@
       <c r="B1" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
@@ -1156,6 +1335,9 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="15">
       <c r="A3" s="1" t="s">
@@ -1239,8 +1421,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
           <x14:formula1>
@@ -1273,14 +1455,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="21.75" customWidth="1"/>
     <col min="2" max="2" width="27.125" customWidth="1"/>
@@ -1299,6 +1481,24 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
@@ -1431,6 +1631,9 @@
       <c r="C7" t="s">
         <v>42</v>
       </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
@@ -1496,6 +1699,9 @@
       <c r="C11" t="s">
         <v>51</v>
       </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
@@ -1507,6 +1713,9 @@
       <c r="C12" t="s">
         <v>50</v>
       </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
@@ -1517,6 +1726,9 @@
       </c>
       <c r="C13" t="s">
         <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
       </c>
       <c r="L13" t="s">
         <v>30</v>
@@ -1530,8 +1742,8 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId1"/>
-  <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de webservice" prompt="Tipo de conexion al servidor">
           <x14:formula1>
@@ -1549,13 +1761,13 @@
           <x14:formula1>
             <xm:f>ZeroCode!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>A13 A4:A6 A8:A10</xm:sqref>
+          <xm:sqref>A4:A13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Es un campo obligatorio?" prompt="Si el campo es obligatorio, seleccione la opcion si, de lo contrario el campo no es obligatorio">
           <x14:formula1>
             <xm:f>ZeroCode!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:E6 E8:E10 D23:D25</xm:sqref>
+          <xm:sqref>E4:E13 D23:D25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de dato" prompt="Selecciona el tipo de dato a recibir">
           <x14:formula1>
@@ -1570,14 +1782,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>
@@ -1609,7 +1821,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1625,10 +1837,10 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
El nombre de la tabla se configura en el nombre de la hoja de calculo, se elimina nombre_tabla Se permite parametrizar si se desea crear la barra de progreso en el formulario, ver hoja de configuracion en hoja de calculo (ZC_CONFIG_INCLUIR_PROGRESO) #58 Se permite parametrizar si se desea crear la barra de navegacion en el formulario, ver hoja de configuracion en hoja de calculo (ZC_CONFIG_INCLUIR_NAVBAR) #58
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="4" r:id="rId1"/>
-    <sheet name="Paises" sheetId="3" r:id="rId2"/>
+    <sheet name="t_Paises" sheetId="3" r:id="rId2"/>
     <sheet name="Clientes" sheetId="1" r:id="rId3"/>
     <sheet name="ZeroCode" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
@@ -501,7 +501,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="98">
   <si>
     <t>Nombre Formulario</t>
   </si>
@@ -767,9 +767,6 @@
     <t>Checkbox</t>
   </si>
   <si>
-    <t>Paises::PaNombre</t>
-  </si>
-  <si>
     <t>WS Agregar</t>
   </si>
   <si>
@@ -788,20 +785,26 @@
     <t>WS Precargar</t>
   </si>
   <si>
-    <t>Nombre tabla</t>
-  </si>
-  <si>
-    <t>t_paises</t>
+    <t>Con login</t>
+  </si>
+  <si>
+    <t>Con barra progreso</t>
+  </si>
+  <si>
+    <t>t_Paises::PaNombre</t>
+  </si>
+  <si>
+    <t>Con navegacion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-240A]#,##0.00;[Red]&quot;(&quot;[$$-240A]#,##0.00&quot;)&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -846,6 +849,12 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -881,9 +890,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -894,16 +904,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -977,7 +982,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1012,7 +1016,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1188,18 +1191,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="15.125" customWidth="1"/>
     <col min="5" max="5" width="14.25" customWidth="1"/>
     <col min="6" max="6" width="14.75" customWidth="1"/>
@@ -1257,50 +1260,45 @@
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
         <v>15</v>
       </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="B5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Base de datos" prompt="Base de datos utilizar, se puede configurar por formulario">
-          <x14:formula1>
-            <xm:f>ZeroCode!$E$2:$E$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>ZeroCode!$F$2:$F$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>ZeroCode!$G$2:$G$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
@@ -1324,9 +1322,6 @@
       <c r="B1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
@@ -1335,9 +1330,6 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="3" spans="1:13" ht="15">
       <c r="A3" s="1" t="s">
@@ -1421,48 +1413,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
-          <x14:formula1>
-            <xm:f>ZeroCode!$A$2:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>A4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Base de datos" prompt="Base de datos utilizar, se puede configurar por formulario">
-          <x14:formula1>
-            <xm:f>ZeroCode!$E$2:$E$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Es un campo obligatorio?" prompt="Si el campo es obligatorio, seleccione la opcion si, de lo contrario el campo no es obligatorio">
-          <x14:formula1>
-            <xm:f>ZeroCode!$C$2:$C$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>E4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de dato" prompt="Selecciona el tipo de dato a recibir">
-          <x14:formula1>
-            <xm:f>ZeroCode!$B$2:$B$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>C4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="21.75" customWidth="1"/>
     <col min="2" max="2" width="27.125" customWidth="1"/>
@@ -1482,22 +1444,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1655,7 +1617,7 @@
         <v>27</v>
       </c>
       <c r="L8" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1742,54 +1704,18 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de webservice" prompt="Tipo de conexion al servidor">
-          <x14:formula1>
-            <xm:f>ZeroCode!$D$2:$D$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Base de datos" prompt="Base de datos utilizar, se puede configurar por formulario">
-          <x14:formula1>
-            <xm:f>ZeroCode!$E$2:$E$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Forma de presentacion del campo" prompt="Solo se permiten los valores de la lista">
-          <x14:formula1>
-            <xm:f>ZeroCode!$A$2:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>A4:A13</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Es un campo obligatorio?" prompt="Si el campo es obligatorio, seleccione la opcion si, de lo contrario el campo no es obligatorio">
-          <x14:formula1>
-            <xm:f>ZeroCode!$C$2:$C$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>E4:E13 D23:D25</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tipo de dato" prompt="Selecciona el tipo de dato a recibir">
-          <x14:formula1>
-            <xm:f>ZeroCode!$B$2:$B$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>C4:C13</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>

</xml_diff>

<commit_message>
e separa la creacion de areas de texto de las cajas de texto eliminando el tipo de dato 'mucho texto' Corregido bug en asignacion de restricciones parsley a elementos tipo: radio y checkbox Se cambia el caracter &[Longitud]& por %s para facilitar el manejo de errores Corregido bug en restriccion de campos no obligatorios no diligenciados del lado servidor, se validaban longitudes
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="4" r:id="rId1"/>
@@ -501,7 +501,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
   <si>
     <t>Nombre Formulario</t>
   </si>
@@ -557,9 +557,6 @@
     <t>Ey! Se te olvido</t>
   </si>
   <si>
-    <t>Muy corto, minimo 5</t>
-  </si>
-  <si>
     <t>Te pasaste</t>
   </si>
   <si>
@@ -572,9 +569,6 @@
     <t>Por favor digita un correo valido</t>
   </si>
   <si>
-    <t>Al menos 10</t>
-  </si>
-  <si>
     <t>Pais</t>
   </si>
   <si>
@@ -593,9 +587,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>1=Si</t>
-  </si>
-  <si>
     <t>fecha</t>
   </si>
   <si>
@@ -668,9 +659,6 @@
     <t>Pagina web</t>
   </si>
   <si>
-    <t>N=Natural,J=Juridica</t>
-  </si>
-  <si>
     <t>Motor BD</t>
   </si>
   <si>
@@ -795,12 +783,33 @@
   </si>
   <si>
     <t>Con navegacion</t>
+  </si>
+  <si>
+    <t>N==Natural||J==Juridica</t>
+  </si>
+  <si>
+    <t>1==Si</t>
+  </si>
+  <si>
+    <t>Numero empleados</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Se acepta minimo %s empleados</t>
+  </si>
+  <si>
+    <t>Al menos %s</t>
+  </si>
+  <si>
+    <t>Muy corto, minimo %s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-240A]#,##0.00;[Red]&quot;(&quot;[$$-240A]#,##0.00&quot;)&quot;"/>
   </numFmts>
@@ -904,11 +913,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -982,6 +996,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1016,6 +1031,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1191,14 +1207,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.125" customWidth="1"/>
@@ -1212,28 +1228,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1241,33 +1257,33 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C2">
         <v>3306</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1291,14 +1307,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
@@ -1320,12 +1336,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1351,7 +1367,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -1366,10 +1382,10 @@
         <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1377,7 +1393,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -1392,22 +1408,22 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" t="s">
         <v>60</v>
       </c>
-      <c r="H4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" t="s">
-        <v>64</v>
-      </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1417,14 +1433,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="21.75" customWidth="1"/>
     <col min="2" max="2" width="27.125" customWidth="1"/>
@@ -1444,27 +1460,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15">
@@ -1487,7 +1503,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -1502,10 +1518,10 @@
         <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1513,7 +1529,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -1528,13 +1544,13 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1542,33 +1558,33 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
       </c>
       <c r="D5">
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -1580,7 +1596,7 @@
         <v>16</v>
       </c>
       <c r="L6" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1588,53 +1604,53 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>100</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1642,10 +1658,10 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -1656,13 +1672,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1670,33 +1686,49 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="K14" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <headerFooter>
@@ -1708,14 +1740,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>
@@ -1726,25 +1758,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1764,86 +1796,86 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizada version de Codeigniter 3.0.6, entre otros widgets js
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="4" r:id="rId1"/>
@@ -501,7 +501,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="102">
   <si>
     <t>Nombre Formulario</t>
   </si>
@@ -804,6 +804,9 @@
   </si>
   <si>
     <t>Muy corto, minimo %s</t>
+  </si>
+  <si>
+    <t>MySQLi</t>
   </si>
 </sst>
 </file>
@@ -1210,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1254,7 +1257,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>67</v>
@@ -1436,7 +1439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1744,7 +1747,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1793,7 +1796,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>101</v>
       </c>
       <c r="F2" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
Corregido bug #75, se causaba por la clase col-xs-12, se quitaron Se mejora compatibilidad con bases de datos en latin1 Por defecto a la funcion init del controlador se leagrega cache de 10 min Se reduce el codigo generado utilizando funciones javascrip genericas     desactivarCampos     activarCampos     ZCRespuestaConError Se cambia funcion ZCAsignarErrores, ya no es necesario el id del formulario Mejorada creacion de script de base de datos
</commit_message>
<xml_diff>
--- a/zc/test/FormatoExcel2007.xlsx
+++ b/zc/test/FormatoExcel2007.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="6855"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="4" r:id="rId1"/>
-    <sheet name="t_Paises" sheetId="3" r:id="rId2"/>
-    <sheet name="Clientes" sheetId="1" r:id="rId3"/>
+    <sheet name="Clientes" sheetId="1" r:id="rId2"/>
+    <sheet name="Paises" sheetId="3" r:id="rId3"/>
     <sheet name="ZeroCode" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -23,55 +23,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Farfan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Este nombre se muestra en el formulario</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Farfan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Tipo de motor de base de datos que se usa para almacenar los datos</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -123,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -175,6 +127,58 @@
         </r>
       </text>
     </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+URL donde se encuentra el WS a consumir, es del tipo:
+soap|http://path/ws
+rest|http://path/ws</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+URL donde se encuentra el WS a consumir, es del tipo:
+soap|http://path/ws
+rest|http://path/ws</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A3" authorId="1">
       <text>
         <r>
@@ -188,6 +192,30 @@
       </text>
     </comment>
     <comment ref="B3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Liberation Sans"/>
+          </rPr>
+          <t>Nombre del elemento, este se mostrara al cliente, ademas es el nombre del campo en la base de datos. Los espacios se reemplazan por _</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A14" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="8"/>
+            <rFont val="Liberation Sans"/>
+          </rPr>
+          <t>Tipo de elemento a crear</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="1">
       <text>
         <r>
           <rPr>
@@ -210,7 +238,55 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Este nombre se muestra en el formulario</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farfan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tipo de motor de base de datos que se usa para almacenar los datos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -236,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -262,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -288,7 +364,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -314,58 +390,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Farfan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-URL donde se encuentra el WS a consumir, es del tipo:
-soap|http://path/ws
-rest|http://path/ws</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Farfan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-URL donde se encuentra el WS a consumir, es del tipo:
-soap|http://path/ws
-rest|http://path/ws</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A3" authorId="1">
       <text>
         <r>
@@ -379,30 +403,6 @@
       </text>
     </comment>
     <comment ref="B3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="8"/>
-            <rFont val="Liberation Sans"/>
-          </rPr>
-          <t>Nombre del elemento, este se mostrara al cliente, ademas es el nombre del campo en la base de datos. Los espacios se reemplazan por _</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A14" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="8"/>
-            <rFont val="Liberation Sans"/>
-          </rPr>
-          <t>Tipo de elemento a crear</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B14" authorId="1">
       <text>
         <r>
           <rPr>
@@ -512,9 +512,6 @@
     <t>SOAP</t>
   </si>
   <si>
-    <t>MySQL</t>
-  </si>
-  <si>
     <t>Que quieres?</t>
   </si>
   <si>
@@ -566,21 +563,12 @@
     <t>correo</t>
   </si>
   <si>
-    <t>Por favor digita un correo valido</t>
-  </si>
-  <si>
-    <t>Pais</t>
-  </si>
-  <si>
     <t>numero</t>
   </si>
   <si>
     <t>Selecciona un valor de la lista</t>
   </si>
   <si>
-    <t>y el pais?</t>
-  </si>
-  <si>
     <t>Recibir publicidad</t>
   </si>
   <si>
@@ -653,12 +641,6 @@
     <t>Hora registro</t>
   </si>
   <si>
-    <t>Ultima actualizacion</t>
-  </si>
-  <si>
-    <t>Pagina web</t>
-  </si>
-  <si>
     <t>Motor BD</t>
   </si>
   <si>
@@ -674,18 +656,6 @@
     <t>Colombia</t>
   </si>
   <si>
-    <t>Se necesitan caracteres</t>
-  </si>
-  <si>
-    <t>Por favor coloca el nombre</t>
-  </si>
-  <si>
-    <t>Ojo la longitud minima</t>
-  </si>
-  <si>
-    <t>Supera la longitud maxima</t>
-  </si>
-  <si>
     <t>Valores</t>
   </si>
   <si>
@@ -779,34 +749,64 @@
     <t>Con barra progreso</t>
   </si>
   <si>
-    <t>t_Paises::PaNombre</t>
-  </si>
-  <si>
     <t>Con navegacion</t>
   </si>
   <si>
-    <t>N==Natural||J==Juridica</t>
-  </si>
-  <si>
     <t>1==Si</t>
   </si>
   <si>
-    <t>Numero empleados</t>
-  </si>
-  <si>
     <t>Area</t>
   </si>
   <si>
-    <t>Se acepta minimo %s empleados</t>
-  </si>
-  <si>
     <t>Al menos %s</t>
   </si>
   <si>
-    <t>Muy corto, minimo %s</t>
-  </si>
-  <si>
     <t>MySQLi</t>
+  </si>
+  <si>
+    <t>País</t>
+  </si>
+  <si>
+    <t>Página web</t>
+  </si>
+  <si>
+    <t>Última actualización</t>
+  </si>
+  <si>
+    <t>Número empleados</t>
+  </si>
+  <si>
+    <t>Por favor digita un correo válido</t>
+  </si>
+  <si>
+    <t>y el país?</t>
+  </si>
+  <si>
+    <t>N==Natural||J==Jurídica</t>
+  </si>
+  <si>
+    <t>Se acepta mínimo %s empleados</t>
+  </si>
+  <si>
+    <t>Ojo la longitud mínima</t>
+  </si>
+  <si>
+    <t>Supera la longitud máxima</t>
+  </si>
+  <si>
+    <t>Se necesitan carácteres</t>
+  </si>
+  <si>
+    <t>Por favor coloca el nombre del país</t>
+  </si>
+  <si>
+    <t>Muy corto, mínimo %s</t>
+  </si>
+  <si>
+    <t>Países</t>
+  </si>
+  <si>
+    <t>Paises::PaNombre</t>
   </si>
 </sst>
 </file>
@@ -1211,10 +1211,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1231,62 +1232,62 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C2">
         <v>3306</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1294,10 +1295,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1311,10 +1312,319 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="21.75" customWidth="1"/>
+    <col min="2" max="2" width="27.125" customWidth="1"/>
+    <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="18.75" customWidth="1"/>
+    <col min="7" max="8" width="29.375" customWidth="1"/>
+    <col min="9" max="9" width="29.75" customWidth="1"/>
+    <col min="10" max="10" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="K14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1339,94 +1649,94 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="J4" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="K4" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="M4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1435,319 +1745,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="21.75" customWidth="1"/>
-    <col min="2" max="2" width="27.125" customWidth="1"/>
-    <col min="3" max="3" width="16.75" customWidth="1"/>
-    <col min="4" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="18.75" customWidth="1"/>
-    <col min="7" max="8" width="29.375" customWidth="1"/>
-    <col min="9" max="9" width="29.75" customWidth="1"/>
-    <col min="10" max="10" width="29.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9">
-        <v>100</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14">
-        <v>10</v>
-      </c>
-      <c r="K14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F3" sqref="F3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1761,124 +1765,124 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="G1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>